<commit_message>
Add surfaces and hpc_logs
</commit_message>
<xml_diff>
--- a/experiments/08_blase3D_HPC_test/hpc_logs.xlsx
+++ b/experiments/08_blase3D_HPC_test/hpc_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sujay\Documents\GitHub\blase3D\experiments\08_blase3D_HPC_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9241A55-4577-45F5-B2D5-8C90207DBA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED385C3E-DD41-4C17-A893-3C6E746E2ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A8A0078E-A607-4A3F-8885-849D7A1F6AAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Run Date</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>11000 - 12000</t>
-  </si>
-  <si>
     <t>142M</t>
   </si>
   <si>
@@ -72,13 +69,64 @@
   </si>
   <si>
     <t>Triton</t>
+  </si>
+  <si>
+    <t>305M</t>
+  </si>
+  <si>
+    <t>Run #</t>
+  </si>
+  <si>
+    <t>Exp #</t>
+  </si>
+  <si>
+    <t>Commit SHA</t>
+  </si>
+  <si>
+    <t>322c3b</t>
+  </si>
+  <si>
+    <t>Grid Points</t>
+  </si>
+  <si>
+    <t>Realized Grid Points</t>
+  </si>
+  <si>
+    <t>Teff Range</t>
+  </si>
+  <si>
+    <t>Logg Range</t>
+  </si>
+  <si>
+    <t>Z Range</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>(-0.5, 0.5)</t>
+  </si>
+  <si>
+    <t>(11000, 12000)</t>
+  </si>
+  <si>
+    <t>(10000, 12500)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Median Std</t>
+  </si>
+  <si>
+    <t>Median Skewness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +141,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -127,6 +182,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -443,82 +507,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C564E0-E7C2-46D4-938B-9ADACE9C8832}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45194</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1964</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1964</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
         <v>45194</v>
       </c>
-      <c r="B3" s="3">
-        <v>4.7222222222222221E-2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D4" s="3">
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1964</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1964</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1">
         <v>6000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="I4" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F3" s="1">
+      <c r="J4" s="1">
         <v>100</v>
       </c>
-      <c r="G3" s="1">
+      <c r="K4" s="1">
         <v>0.5</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>